<commit_message>
try to keep style as possible
</commit_message>
<xml_diff>
--- a/testdata/excel_test_divide.xlsx
+++ b/testdata/excel_test_divide.xlsx
@@ -31,12 +31,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>target sheet</t>
   </si>
   <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>Mine</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -49,7 +58,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +69,12 @@
     <font>
       <sz val="24"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -209,7 +224,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +233,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -279,12 +312,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -529,88 +556,82 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -619,10 +640,10 @@
     <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -631,10 +652,10 @@
     <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -643,10 +664,10 @@
     <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -655,19 +676,43 @@
     <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1194,30 +1239,35 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" s="8" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1240,21 +1290,21 @@
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
+      <c r="A1" s="3" t="s">
+        <v>2</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1268,30 +1318,35 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1314,21 +1369,21 @@
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
+      <c r="A1" s="3" t="s">
+        <v>2</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1342,13 +1397,13 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -1366,6 +1421,11 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>